<commit_message>
Completed sign up validations
</commit_message>
<xml_diff>
--- a/IncuByte testcases.xlsx
+++ b/IncuByte testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santh\Desktop\IncuByte Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB1953D-B34A-488E-9BD7-0DBC9962E48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A234DD2B-BCFF-4797-B42F-AB08CE46D26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{9A756D2D-C22C-4AA1-A73C-A7C9D9BAB841}"/>
   </bookViews>
@@ -60,11 +60,6 @@
   </si>
   <si>
     <t>User lands on create account page.
-User provides all valid details and submits form.
-New account is created and user is redirected to account page.</t>
-  </si>
-  <si>
-    <t>User lands on create account page.
 User submits registration form with no details.
 New account is not created and errors are displayed</t>
   </si>
@@ -114,6 +109,12 @@
     <t>User lands on create account page.
 User enters password with length more than 8 
 password strength is weak and error is displayed</t>
+  </si>
+  <si>
+    <t>User lands on create account page.
+User provides all valid details and submits form.
+New account is created and user is redirected to account page.
+User is able to login using new account detials</t>
   </si>
 </sst>
 </file>
@@ -479,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEDDB573-3F7E-4E1A-8692-A325A3CB5E4C}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -512,7 +513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -520,7 +521,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
@@ -531,7 +532,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
@@ -539,10 +540,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="87" x14ac:dyDescent="0.35">
@@ -550,10 +551,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="87" x14ac:dyDescent="0.35">
@@ -561,10 +562,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
@@ -572,10 +573,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
@@ -583,10 +584,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
@@ -594,10 +595,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>